<commit_message>
feat: random order columns support
</commit_message>
<xml_diff>
--- a/CodeAndExample/Database.xlsx
+++ b/CodeAndExample/Database.xlsx
@@ -1,14 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24288" windowHeight="11016"/>
+  </bookViews>
   <sheets>
-    <sheet sheetId="1" name="Actors" state="visible" r:id="rId4"/>
-    <sheet sheetId="2" name="Enemies" state="visible" r:id="rId5"/>
-    <sheet sheetId="3" name="Weapons" state="visible" r:id="rId6"/>
+    <sheet name="Actors" sheetId="1" r:id="rId1"/>
+    <sheet name="Enemies" sheetId="2" r:id="rId2"/>
+    <sheet name="Weapons" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -2407,13 +2410,20 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
-      <sz val="11"/>
-      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -2440,7 +2450,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2456,7 +2466,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2466,44 +2476,44 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="1F497D"/>
+        <a:srgbClr val="44546A"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="EEECE1"/>
+        <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4F81BD"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="C0504D"/>
+        <a:srgbClr val="ED7D31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="9BBB59"/>
+        <a:srgbClr val="A5A5A5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="8064A2"/>
+        <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4BACC6"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="F79646"/>
+        <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0000FF"/>
+        <a:srgbClr val="0563C1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="800080"/>
+        <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -2533,12 +2543,12 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -2577,320 +2587,258 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="35000">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="100000"/>
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
                 <a:shade val="100000"/>
-                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:shade val="100000"/>
-                <a:satMod val="350000"/>
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
+                <a:alpha val="63000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
-          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-                <a:satMod val="350000"/>
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="40000">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-                <a:satMod val="350000"/>
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
-                <a:satMod val="255000"/>
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
-                <a:satMod val="200000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults>
-    <a:spDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="3">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </a:style>
-    </a:spDef>
-    <a:lnDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </a:style>
-    </a:lnDef>
-  </a:objectDefaults>
+  <a:objectDefaults/>
   <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U6"/>
+  <dimension ref="A1:V6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
+        <v>99</v>
+      </c>
+      <c r="C2">
         <v>1</v>
       </c>
-      <c r="C2">
-        <v>99</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>21</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>2</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>22</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>23</v>
       </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
       <c r="I2">
         <v>0</v>
       </c>
       <c r="J2">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="K2">
         <v>50</v>
       </c>
       <c r="L2">
+        <v>50</v>
+      </c>
+      <c r="M2">
         <v>2</v>
       </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
       <c r="N2">
         <v>0</v>
       </c>
@@ -2900,7 +2848,7 @@
       <c r="P2">
         <v>0</v>
       </c>
-      <c r="Q2" t="b">
+      <c r="Q2">
         <v>0</v>
       </c>
       <c r="R2" t="b">
@@ -2915,47 +2863,47 @@
       <c r="U2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
+        <v>99</v>
+      </c>
+      <c r="C3">
         <v>1</v>
       </c>
-      <c r="C3">
-        <v>99</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>24</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>3</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>25</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>26</v>
       </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
       <c r="I3">
         <v>0</v>
       </c>
       <c r="J3">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="K3">
         <v>50</v>
       </c>
       <c r="L3">
+        <v>50</v>
+      </c>
+      <c r="M3">
         <v>26</v>
       </c>
-      <c r="M3">
-        <v>0</v>
-      </c>
       <c r="N3">
         <v>0</v>
       </c>
@@ -2965,7 +2913,7 @@
       <c r="P3">
         <v>0</v>
       </c>
-      <c r="Q3" t="b">
+      <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3" t="b">
@@ -2980,47 +2928,47 @@
       <c r="U3" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
+        <v>99</v>
+      </c>
+      <c r="C4">
         <v>1</v>
       </c>
-      <c r="C4">
-        <v>99</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>27</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>4</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>28</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>29</v>
       </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
       <c r="I4">
         <v>0</v>
       </c>
       <c r="J4">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="K4">
         <v>50</v>
       </c>
       <c r="L4">
+        <v>50</v>
+      </c>
+      <c r="M4">
         <v>14</v>
       </c>
-      <c r="M4">
-        <v>0</v>
-      </c>
       <c r="N4">
         <v>0</v>
       </c>
@@ -3030,7 +2978,7 @@
       <c r="P4">
         <v>0</v>
       </c>
-      <c r="Q4" t="b">
+      <c r="Q4">
         <v>0</v>
       </c>
       <c r="R4" t="b">
@@ -3045,47 +2993,47 @@
       <c r="U4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
+        <v>99</v>
+      </c>
+      <c r="C5">
         <v>1</v>
       </c>
-      <c r="C5">
-        <v>99</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>30</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>5</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>31</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>32</v>
       </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
       <c r="I5">
         <v>0</v>
       </c>
       <c r="J5">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="K5">
         <v>50</v>
       </c>
       <c r="L5">
+        <v>50</v>
+      </c>
+      <c r="M5">
         <v>38</v>
       </c>
-      <c r="M5">
-        <v>0</v>
-      </c>
       <c r="N5">
         <v>0</v>
       </c>
@@ -3095,7 +3043,7 @@
       <c r="P5">
         <v>0</v>
       </c>
-      <c r="Q5" t="b">
+      <c r="Q5">
         <v>0</v>
       </c>
       <c r="R5" t="b">
@@ -3110,43 +3058,43 @@
       <c r="U5" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
+        <v>99</v>
+      </c>
+      <c r="C6">
         <v>1</v>
       </c>
-      <c r="C6">
-        <v>99</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>21</v>
       </c>
-      <c r="E6">
-        <v>50</v>
-      </c>
-      <c r="F6" t="s">
+      <c r="F6">
+        <v>50</v>
+      </c>
+      <c r="G6" t="s">
         <v>22</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>23</v>
       </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
       <c r="I6">
         <v>0</v>
       </c>
       <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
         <v>40</v>
       </c>
-      <c r="K6">
-        <v>50</v>
-      </c>
       <c r="L6">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="M6">
         <v>0</v>
@@ -3160,7 +3108,7 @@
       <c r="P6">
         <v>0</v>
       </c>
-      <c r="Q6" t="b">
+      <c r="Q6">
         <v>0</v>
       </c>
       <c r="R6" t="b">
@@ -3175,10 +3123,14 @@
       <c r="U6" t="b">
         <v>0</v>
       </c>
+      <c r="V6" t="b">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
+  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3191,7 +3143,7 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -37262,8 +37214,9 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
+  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="4294967295" verticalDpi="4294967295"/>
 </worksheet>
 </file>
 
@@ -37276,7 +37229,7 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -59323,7 +59276,8 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
+  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="4294967295" verticalDpi="4294967295"/>
 </worksheet>
 </file>
</xml_diff>